<commit_message>
vault backup: 2023-11-26 12:00:34
Affected files:
0. Attach/0.5 Archives/Evaluation Result.xlsx
</commit_message>
<xml_diff>
--- a/0. Attach/0.5 Archives/Evaluation Result.xlsx
+++ b/0. Attach/0.5 Archives/Evaluation Result.xlsx
@@ -8,17 +8,87 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuming\Documents\MateNote\0. Attach\0.5 Archives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E2C93E-6826-4C29-ABD7-1B73F695D113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51999DD-8987-4F04-AEFE-6C87EE3EF167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6440" yWindow="4140" windowWidth="28800" windowHeight="15560" activeTab="3" xr2:uid="{29E27A0B-FB5E-410D-B37C-BA3847E1800A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" activeTab="5" xr2:uid="{29E27A0B-FB5E-410D-B37C-BA3847E1800A}"/>
   </bookViews>
   <sheets>
     <sheet name="Random" sheetId="1" r:id="rId1"/>
     <sheet name="Fixed" sheetId="2" r:id="rId2"/>
     <sheet name="PPO" sheetId="3" r:id="rId3"/>
     <sheet name="PPO+LTSM" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Result" sheetId="5" r:id="rId5"/>
+    <sheet name="10" sheetId="7" r:id="rId6"/>
+    <sheet name="20" sheetId="8" r:id="rId7"/>
+    <sheet name="40" sheetId="9" r:id="rId8"/>
+    <sheet name="Preparation" sheetId="6" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Random!$C$2:$C$11</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Random!$C$2:$C$30</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'10'!$A$10:$P$10</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'10'!$A$11:$P$11</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'10'!$A$12:$P$12</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'10'!$A$13:$P$13</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'10'!$A$14:$P$14</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'10'!$A$15:$P$15</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'10'!$A$16:$P$16</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'10'!$A$17:$P$17</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'10'!$A$18:$P$18</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'10'!$A$2:$P$2</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Random!$D$2:$D$11</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'10'!$A$3:$P$3</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'10'!$A$4:$P$4</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'10'!$A$5:$P$5</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'10'!$A$6:$P$6</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">'10'!$A$7:$P$7</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">'10'!$A$8:$P$8</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">'10'!$A$9:$P$9</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">'10'!$P$18</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">'10'!$A$10:$P$10</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">'10'!$A$11:$P$11</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Random!$D$2:$D$30</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">'10'!$A$12:$P$12</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">'10'!$A$13:$P$13</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">'10'!$A$14:$P$14</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">'10'!$A$15:$P$15</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">'10'!$A$16:$P$16</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">'10'!$A$17:$P$17</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">'10'!$A$18:$P$18</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">'10'!$A$2:$P$2</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">'10'!$A$3:$P$3</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">'10'!$A$4:$P$4</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Random!$E$2:$E$11</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">'10'!$A$5:$P$5</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">'10'!$A$6:$P$6</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">'10'!$A$7:$P$7</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">'10'!$A$8:$P$8</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">'10'!$A$9:$P$9</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">'10'!$P$18</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">'10'!$A$10:$P$10</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">'10'!$A$11:$P$11</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">'10'!$A$12:$P$12</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">'10'!$A$13:$P$13</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Random!$E$2:$E$30</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">'10'!$A$14:$P$14</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">'10'!$A$15:$P$15</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">'10'!$A$16:$P$16</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">'10'!$A$17:$P$17</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">'10'!$A$18:$P$18</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">'10'!$A$2:$P$2</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">'10'!$A$3:$P$3</definedName>
+    <definedName name="_xlchart.v1.57" hidden="1">'10'!$A$4:$P$4</definedName>
+    <definedName name="_xlchart.v1.58" hidden="1">'10'!$A$5:$P$5</definedName>
+    <definedName name="_xlchart.v1.59" hidden="1">'10'!$A$6:$P$6</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Random!$F$2:$F$11</definedName>
+    <definedName name="_xlchart.v1.60" hidden="1">'10'!$A$7:$P$7</definedName>
+    <definedName name="_xlchart.v1.61" hidden="1">'10'!$A$8:$P$8</definedName>
+    <definedName name="_xlchart.v1.62" hidden="1">'10'!$A$9:$P$9</definedName>
+    <definedName name="_xlchart.v1.63" hidden="1">'10'!$P$18</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Random!$F$2:$F$30</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Random!$F$30</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'10'!$P$18</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="64">
   <si>
     <t>Total Job</t>
   </si>
@@ -125,18 +195,6 @@
     <t>0.908201430142582±0.00708275135876675</t>
   </si>
   <si>
-    <t>2824175.23356443±296.277741317163</t>
-  </si>
-  <si>
-    <t>1143300.93944946±37898.4247399774</t>
-  </si>
-  <si>
-    <t>0.268890945039438±0.00536969261750618</t>
-  </si>
-  <si>
-    <t>0.779141932974332±0.0120117763001532</t>
-  </si>
-  <si>
     <t>PPO+LTSM</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -177,23 +235,90 @@
     <t>0.721292389156887±0.00949577928541033</t>
   </si>
   <si>
-    <t>4865873.6566243±102559.036377258</t>
-  </si>
-  <si>
-    <t>1636792.36105183±25820.0134762105</t>
-  </si>
-  <si>
-    <t>0.23578700484147±0.00416128711147407</t>
-  </si>
-  <si>
-    <t>0.633188669289859±0.00744780298799901</t>
+    <t>3061859.83565773±88.3883476483184</t>
+  </si>
+  <si>
+    <t>1619990.59598074±35646.8909253565</t>
+  </si>
+  <si>
+    <t>0.214934049476589±0.00627561068500619</t>
+  </si>
+  <si>
+    <t>0.9281766984137±0.00933700321547977</t>
+  </si>
+  <si>
+    <t>4659271.90165733±100026.576065109</t>
+  </si>
+  <si>
+    <t>2341607.26615135±43607.6325482302</t>
+  </si>
+  <si>
+    <t>0.203469422892037±0.00638336911148005</t>
+  </si>
+  <si>
+    <t>0.734267509339621±0.0102137348480835</t>
+  </si>
+  <si>
+    <t>1462740.155±69033.1420375868</t>
+  </si>
+  <si>
+    <t>545493.514830869±36741.6904057123</t>
+  </si>
+  <si>
+    <t>0.190782756514891±0.011580191640062</t>
+  </si>
+  <si>
+    <t>0.756605965550828±0.0135272734535628</t>
+  </si>
+  <si>
+    <t>1598052.095±81909.5620785324</t>
+  </si>
+  <si>
+    <t>759758.930866268±47283.1068698491</t>
+  </si>
+  <si>
+    <t>0.199420598159134±0.00538671191049339</t>
+  </si>
+  <si>
+    <t>0.914462159217786±0.00987479813764537</t>
+  </si>
+  <si>
+    <t>1494683.66263474±59890.9885505285</t>
+  </si>
+  <si>
+    <t>780211.123011167±35794.0092236306</t>
+  </si>
+  <si>
+    <t>0.20308524058952±0.0110048031353373</t>
+  </si>
+  <si>
+    <t>0.924640071955547±0.00956310055231205</t>
+  </si>
+  <si>
+    <t>1526728.92401679±81088.5388601975</t>
+  </si>
+  <si>
+    <t>824693.78316413±63173.0398867113</t>
+  </si>
+  <si>
+    <t>0.179818459648584±0.0104481614154343</t>
+  </si>
+  <si>
+    <t>0.933924001342734±0.0119481581570159</t>
+  </si>
+  <si>
+    <t>Complete Rate</t>
+  </si>
+  <si>
+    <t>PPO_LTSM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +337,21 @@
       <sz val="9"/>
       <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF3B3B3B"/>
+      <name val="Cascadia Code"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -238,18 +378,34 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -579,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEB75B47-34C0-4D1B-A289-611307C156F5}">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P11"/>
+      <selection activeCell="S1" sqref="S1:V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -590,7 +746,7 @@
     <col min="3" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -609,11 +765,44 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
       <c r="N1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="Q1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1951</v>
       </c>
@@ -668,8 +857,12 @@
       <c r="U2">
         <v>0.19440940678355501</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V2">
+        <f>R2/Q2</f>
+        <v>0.76007677543186181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1951</v>
       </c>
@@ -724,8 +917,12 @@
       <c r="U3">
         <v>0.18172517842192101</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V3">
+        <f t="shared" ref="V3:V11" si="2">R3/Q3</f>
+        <v>0.75815738963531665</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2040</v>
       </c>
@@ -780,8 +977,12 @@
       <c r="U4">
         <v>0.18260263406496399</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V4">
+        <f t="shared" si="2"/>
+        <v>0.76848249027237359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2040</v>
       </c>
@@ -836,8 +1037,12 @@
       <c r="U5">
         <v>0.189200126990379</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V5">
+        <f t="shared" si="2"/>
+        <v>0.77626459143968873</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2064</v>
       </c>
@@ -892,8 +1097,12 @@
       <c r="U6">
         <v>0.211900232139585</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V6">
+        <f t="shared" si="2"/>
+        <v>0.75948196114708599</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2064</v>
       </c>
@@ -948,8 +1157,12 @@
       <c r="U7">
         <v>0.18973997598287101</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V7">
+        <f t="shared" si="2"/>
+        <v>0.72987974098057351</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1976</v>
       </c>
@@ -1004,8 +1217,12 @@
       <c r="U8">
         <v>0.20433769927769299</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V8">
+        <f t="shared" si="2"/>
+        <v>0.73917421953675733</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1976</v>
       </c>
@@ -1060,8 +1277,12 @@
       <c r="U9">
         <v>0.19867457442367001</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V9">
+        <f t="shared" si="2"/>
+        <v>0.75730110775427995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1952</v>
       </c>
@@ -1116,8 +1337,12 @@
       <c r="U10">
         <v>0.178773811895486</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V10">
+        <f t="shared" si="2"/>
+        <v>0.75270935960591134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1952</v>
       </c>
@@ -1172,8 +1397,12 @@
       <c r="U11">
         <v>0.17646392516878101</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V11">
+        <f t="shared" si="2"/>
+        <v>0.76453201970443352</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -1181,15 +1410,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="4">
         <f>AVERAGEA(C2:C11)</f>
         <v>2738808.6424999973</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <f>STDEV(A2:B2)</f>
         <v>357.08892449920648</v>
       </c>
@@ -1197,104 +1426,152 @@
         <f>B16&amp;"±"&amp;C16</f>
         <v>2738808.6425±357.088924499206</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="4">
         <f>AVERAGEA(K2:K11)</f>
         <v>4802908.6249999972</v>
       </c>
-      <c r="K16">
-        <f>STDEV(K2:K11)</f>
-        <v>99293.821642515963</v>
+      <c r="K16" s="4">
+        <f>STDEV(I2:J2)</f>
+        <v>1003.384522503711</v>
       </c>
       <c r="L16" t="str">
         <f>J16&amp;"±"&amp;K16</f>
-        <v>4802908.625±99293.821642516</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+        <v>4802908.625±1003.38452250371</v>
+      </c>
+      <c r="R16" s="4">
+        <f>AVERAGEA(S2:S11)</f>
+        <v>1462740.1549999961</v>
+      </c>
+      <c r="S16" s="4">
+        <f>STDEV(Q2:R2)</f>
+        <v>176.77669529663689</v>
+      </c>
+      <c r="T16" t="str">
+        <f>R16&amp;"±"&amp;S16</f>
+        <v>1462740.155±176.776695296637</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="4">
         <f>AVERAGEA(D2:D11)</f>
         <v>989836.85921313427</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <f>STDEV(D2:D11)</f>
         <v>32953.003434453109</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" ref="D17:D19" si="2">B17&amp;"±"&amp;C17</f>
+        <f t="shared" ref="D17:D19" si="3">B17&amp;"±"&amp;C17</f>
         <v>989836.859213134±32953.0034344531</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="4">
         <f>AVERAGEA(L2:L11)</f>
         <v>1635198.847215984</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="4">
         <f>STDEV(L2:L11)</f>
         <v>34407.863752007033</v>
       </c>
       <c r="L17" t="str">
-        <f t="shared" ref="L17:L19" si="3">J17&amp;"±"&amp;K17</f>
+        <f t="shared" ref="L17:L19" si="4">J17&amp;"±"&amp;K17</f>
         <v>1635198.84721598±34407.863752007</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="R17" s="4">
+        <f>AVERAGEA(T2:T11)</f>
+        <v>545493.51483086904</v>
+      </c>
+      <c r="S17" s="4">
+        <f>STDEV(T2:T11)</f>
+        <v>36741.690405712332</v>
+      </c>
+      <c r="T17" t="str">
+        <f t="shared" ref="T17:T19" si="5">R17&amp;"±"&amp;S17</f>
+        <v>545493.514830869±36741.6904057123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="4">
         <f>AVERAGEA(E2:E11)</f>
         <v>0.21548607607772174</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <f>STDEV(E2:E11)</f>
         <v>6.5165687431125319E-3</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.215486076077722±0.00651656874311253</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="4">
         <f>AVERAGEA(M2:M11)</f>
         <v>0.21587670171373255</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="4">
         <f>STDEV(M2:M11)</f>
         <v>5.6959869156377983E-3</v>
       </c>
       <c r="L18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.215876701713733±0.0056959869156378</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="R18" s="4">
+        <f>AVERAGEA(U2:U11)</f>
+        <v>0.19078275651489052</v>
+      </c>
+      <c r="S18" s="4">
+        <f>STDEV(U2:U11)</f>
+        <v>1.158019164006199E-2</v>
+      </c>
+      <c r="T18" t="str">
+        <f t="shared" si="5"/>
+        <v>0.190782756514891±0.011580191640062</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="4">
         <f>AVERAGEA(F2:F11)</f>
         <v>0.72430956222185217</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="4">
         <f>STDEV(F2:F11)</f>
         <v>8.3239442963862417E-3</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.724309562221852±0.00832394429638624</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="4">
         <f>AVERAGEA(N2:N11)</f>
         <v>0.6291547871134775</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="4">
         <f>STDEV(N2:N11)</f>
         <v>6.9314266675382591E-3</v>
       </c>
       <c r="L19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.629154787113477±0.00693142666753826</v>
+      </c>
+      <c r="R19" s="4">
+        <f>AVERAGEA(V2:V11)</f>
+        <v>0.75660596555082826</v>
+      </c>
+      <c r="S19" s="4">
+        <f>STDEV(V2:V11)</f>
+        <v>1.3527273453562819E-2</v>
+      </c>
+      <c r="T19" t="str">
+        <f t="shared" si="5"/>
+        <v>0.756605965550828±0.0135272734535628</v>
       </c>
     </row>
   </sheetData>
@@ -1306,15 +1583,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B5BF83-EBB1-4200-87B2-A1FD8CF17F86}">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P11"/>
+      <selection activeCell="S1" sqref="S1:V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1333,11 +1610,44 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
       <c r="N1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="Q1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1951</v>
       </c>
@@ -1392,8 +1702,12 @@
       <c r="U2">
         <v>0.189500472648126</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V2">
+        <f>R2/Q2</f>
+        <v>0.89923224568138194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1951</v>
       </c>
@@ -1448,8 +1762,12 @@
       <c r="U3">
         <v>0.189500472648126</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V3">
+        <f t="shared" ref="V3:V11" si="2">R3/Q3</f>
+        <v>0.89923224568138194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2040</v>
       </c>
@@ -1504,8 +1822,12 @@
       <c r="U4">
         <v>0.20409025312008999</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V4">
+        <f t="shared" si="2"/>
+        <v>0.91828793774319062</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2040</v>
       </c>
@@ -1560,8 +1882,12 @@
       <c r="U5">
         <v>0.20409025312008999</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V5">
+        <f t="shared" si="2"/>
+        <v>0.91828793774319062</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2064</v>
       </c>
@@ -1616,8 +1942,12 @@
       <c r="U6">
         <v>0.20102213679338099</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V6">
+        <f t="shared" si="2"/>
+        <v>0.92229417206290476</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2064</v>
       </c>
@@ -1672,8 +2002,12 @@
       <c r="U7">
         <v>0.20102213679338099</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V7">
+        <f t="shared" si="2"/>
+        <v>0.92229417206290476</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1976</v>
       </c>
@@ -1728,8 +2062,12 @@
       <c r="U8">
         <v>0.20199943397371101</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V8">
+        <f t="shared" si="2"/>
+        <v>0.90835850956696873</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1976</v>
       </c>
@@ -1784,8 +2122,12 @@
       <c r="U9">
         <v>0.20199943397371101</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V9">
+        <f t="shared" si="2"/>
+        <v>0.90835850956696873</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1952</v>
       </c>
@@ -1840,8 +2182,12 @@
       <c r="U10">
         <v>0.20049069426036401</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V10">
+        <f t="shared" si="2"/>
+        <v>0.92413793103448272</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1952</v>
       </c>
@@ -1896,8 +2242,12 @@
       <c r="U11">
         <v>0.20049069426036401</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V11">
+        <f t="shared" si="2"/>
+        <v>0.92413793103448272</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -1905,15 +2255,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="4">
         <f>AVERAGEA(C2:C11)</f>
         <v>3048057.26</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <f>STDEV(A2:B2)</f>
         <v>141.42135623730951</v>
       </c>
@@ -1921,104 +2271,152 @@
         <f>B16&amp;"±"&amp;C16</f>
         <v>3048057.26±141.42135623731</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="4">
         <f>AVERAGEA(K2:K11)</f>
         <v>4732284.4549999963</v>
       </c>
-      <c r="K16">
-        <f>STDEV(K2:K11)</f>
-        <v>46297.609810271191</v>
+      <c r="K16" s="4">
+        <f>STDEV(I2:J2)</f>
+        <v>707.10678118654755</v>
       </c>
       <c r="L16" t="str">
         <f>J16&amp;"±"&amp;K16</f>
-        <v>4732284.455±46297.6098102712</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+        <v>4732284.455±707.106781186548</v>
+      </c>
+      <c r="R16" s="4">
+        <f>AVERAGEA(S2:S11)</f>
+        <v>1598052.0949999962</v>
+      </c>
+      <c r="S16" s="4">
+        <f>STDEV(Q2:R2)</f>
+        <v>74.246212024587493</v>
+      </c>
+      <c r="T16" t="str">
+        <f>R16&amp;"±"&amp;S16</f>
+        <v>1598052.095±74.2462120245875</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="4">
         <f>AVERAGEA(D2:D11)</f>
         <v>1434300.0029287382</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <f>STDEV(D2:D11)</f>
         <v>40277.863881067722</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" ref="D17:D19" si="2">B17&amp;"±"&amp;C17</f>
+        <f t="shared" ref="D17:D19" si="3">B17&amp;"±"&amp;C17</f>
         <v>1434300.00292874±40277.8638810677</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="4">
         <f>AVERAGEA(L2:L11)</f>
         <v>2259543.1110879816</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="4">
         <f>STDEV(L2:L11)</f>
         <v>33823.705830680825</v>
       </c>
       <c r="L17" t="str">
-        <f t="shared" ref="L17:L19" si="3">J17&amp;"±"&amp;K17</f>
+        <f t="shared" ref="L17:L19" si="4">J17&amp;"±"&amp;K17</f>
         <v>2259543.11108798±33823.7058306808</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="R17" s="4">
+        <f>AVERAGEA(T2:T11)</f>
+        <v>759758.93086626811</v>
+      </c>
+      <c r="S17" s="4">
+        <f>STDEV(T2:T11)</f>
+        <v>47283.106869849136</v>
+      </c>
+      <c r="T17" t="str">
+        <f t="shared" ref="T17:T19" si="5">R17&amp;"±"&amp;S17</f>
+        <v>759758.930866268±47283.1068698491</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="4">
         <f>AVERAGEA(E2:E11)</f>
         <v>0.22762501801438279</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <f>STDEV(E2:E11)</f>
         <v>4.2830428184726281E-3</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.227625018014383±0.00428304281847263</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="4">
         <f>AVERAGEA(M2:M11)</f>
         <v>0.20628624026275938</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="4">
         <f>STDEV(M2:M11)</f>
         <v>4.3282706953054195E-3</v>
       </c>
       <c r="L18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.206286240262759±0.00432827069530542</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="R18" s="4">
+        <f>AVERAGEA(U2:U11)</f>
+        <v>0.19942059815913438</v>
+      </c>
+      <c r="S18" s="4">
+        <f>STDEV(U2:U11)</f>
+        <v>5.3867119104933905E-3</v>
+      </c>
+      <c r="T18" t="str">
+        <f t="shared" si="5"/>
+        <v>0.199420598159134±0.00538671191049339</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="4">
         <f>AVERAGEA(F2:F11)</f>
         <v>0.90106095121144192</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="4">
         <f>STDEV(F2:F11)</f>
         <v>5.3188975887088425E-3</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.901060951211442±0.00531889758870884</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="4">
         <f>AVERAGEA(N2:N11)</f>
         <v>0.73206688215105165</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="4">
         <f>STDEV(N2:N11)</f>
         <v>9.3834181513469377E-3</v>
       </c>
       <c r="L19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.732066882151052±0.00938341815134694</v>
+      </c>
+      <c r="R19" s="4">
+        <f>AVERAGEA(V2:V11)</f>
+        <v>0.91446215921778595</v>
+      </c>
+      <c r="S19" s="4">
+        <f>STDEV(V2:V11)</f>
+        <v>9.8747981376453731E-3</v>
+      </c>
+      <c r="T19" t="str">
+        <f t="shared" si="5"/>
+        <v>0.914462159217786±0.00987479813764537</v>
       </c>
     </row>
   </sheetData>
@@ -2030,10 +2428,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A7C1F1-FE29-455B-BE26-E171979D3D8A}">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P11"/>
+      <selection activeCell="S1" sqref="S1:V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2046,7 +2444,7 @@
     <col min="7" max="7" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2065,11 +2463,44 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
       <c r="N1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="Q1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1937</v>
       </c>
@@ -2124,8 +2555,12 @@
       <c r="U2">
         <v>0.18791067091586899</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V2">
+        <f>R2/Q2</f>
+        <v>0.93561786085150567</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1982</v>
       </c>
@@ -2180,8 +2615,12 @@
       <c r="U3">
         <v>0.20416533663966499</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V3">
+        <f t="shared" ref="V3:V11" si="2">R3/Q3</f>
+        <v>0.9198355601233299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2031</v>
       </c>
@@ -2236,8 +2675,12 @@
       <c r="U4">
         <v>0.188271171503227</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V4">
+        <f t="shared" si="2"/>
+        <v>0.92484342379958251</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2026</v>
       </c>
@@ -2292,8 +2735,12 @@
       <c r="U5">
         <v>0.20946071415717499</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V5">
+        <f t="shared" si="2"/>
+        <v>0.92315789473684207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1989</v>
       </c>
@@ -2348,8 +2795,12 @@
       <c r="U6">
         <v>0.19424720963258499</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V6">
+        <f t="shared" si="2"/>
+        <v>0.94094094094094094</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1995</v>
       </c>
@@ -2404,8 +2855,12 @@
       <c r="U7">
         <v>0.204147805857886</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V7">
+        <f t="shared" si="2"/>
+        <v>0.90861344537815125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2079</v>
       </c>
@@ -2460,8 +2915,12 @@
       <c r="U8">
         <v>0.211465497033552</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V8">
+        <f t="shared" si="2"/>
+        <v>0.92162698412698407</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1951</v>
       </c>
@@ -2516,8 +2975,12 @@
       <c r="U9">
         <v>0.20595657710041301</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V9">
+        <f t="shared" si="2"/>
+        <v>0.91412213740458015</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2024</v>
       </c>
@@ -2572,8 +3035,12 @@
       <c r="U10">
         <v>0.20123133203839999</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V10">
+        <f t="shared" si="2"/>
+        <v>0.92884990253411304</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1960</v>
       </c>
@@ -2628,8 +3095,12 @@
       <c r="U11">
         <v>0.223996091016432</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V11">
+        <f t="shared" si="2"/>
+        <v>0.92879256965944268</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -2637,15 +3108,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="4">
         <f>AVERAGEA(C2:C11)</f>
         <v>2952585.167493639</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <f>STDEV(A2:B2)</f>
         <v>108.18733752154178</v>
       </c>
@@ -2653,104 +3124,152 @@
         <f>B16&amp;"±"&amp;C16</f>
         <v>2952585.16749364±108.187337521542</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="4">
         <f>AVERAGEA(K2:K11)</f>
         <v>4679116.6808595005</v>
       </c>
-      <c r="K16">
-        <f>STDEV(K2:K11)</f>
-        <v>95686.539654515989</v>
+      <c r="K16" s="4">
+        <f>STDEV(I2:J2)</f>
+        <v>773.57481861808299</v>
       </c>
       <c r="L16" t="str">
         <f>J16&amp;"±"&amp;K16</f>
-        <v>4679116.6808595±95686.539654516</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+        <v>4679116.6808595±773.574818618083</v>
+      </c>
+      <c r="R16" s="4">
+        <f>AVERAGEA(S2:S11)</f>
+        <v>1494683.6626347429</v>
+      </c>
+      <c r="S16" s="4">
+        <f>STDEV(Q2:R2)</f>
+        <v>43.840620433565945</v>
+      </c>
+      <c r="T16" t="str">
+        <f>R16&amp;"±"&amp;S16</f>
+        <v>1494683.66263474±43.8406204335659</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="4">
         <f>AVERAGEA(D2:D11)</f>
         <v>1531590.1294724301</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <f>STDEV(D2:D11)</f>
         <v>60090.040594452577</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" ref="D17:D19" si="2">B17&amp;"±"&amp;C17</f>
+        <f t="shared" ref="D17:D19" si="3">B17&amp;"±"&amp;C17</f>
         <v>1531590.12947243±60090.0405944526</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="4">
         <f>AVERAGEA(L2:L11)</f>
         <v>2292832.5996192796</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="4">
         <f>STDEV(L2:L11)</f>
         <v>53486.977246856877</v>
       </c>
       <c r="L17" t="str">
-        <f t="shared" ref="L17:L19" si="3">J17&amp;"±"&amp;K17</f>
+        <f t="shared" ref="L17:L19" si="4">J17&amp;"±"&amp;K17</f>
         <v>2292832.59961928±53486.9772468569</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="R17" s="4">
+        <f>AVERAGEA(T2:T11)</f>
+        <v>780211.12301116739</v>
+      </c>
+      <c r="S17" s="4">
+        <f>STDEV(T2:T11)</f>
+        <v>35794.009223630637</v>
+      </c>
+      <c r="T17" t="str">
+        <f t="shared" ref="T17:T19" si="5">R17&amp;"±"&amp;S17</f>
+        <v>780211.123011167±35794.0092236306</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="4">
         <f>AVERAGEA(E2:E11)</f>
         <v>0.2177372797011336</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <f>STDEV(E2:E11)</f>
         <v>6.6346499075217733E-3</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.217737279701134±0.00663464990752177</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="4">
         <f>AVERAGEA(M2:M11)</f>
         <v>0.20568538801594505</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="4">
         <f>STDEV(M2:M11)</f>
         <v>3.4581971274630246E-3</v>
       </c>
       <c r="L18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.205685388015945±0.00345819712746302</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="R18" s="4">
+        <f>AVERAGEA(U2:U11)</f>
+        <v>0.2030852405895204</v>
+      </c>
+      <c r="S18" s="4">
+        <f>STDEV(U2:U11)</f>
+        <v>1.100480313533729E-2</v>
+      </c>
+      <c r="T18" t="str">
+        <f t="shared" si="5"/>
+        <v>0.20308524058952±0.0110048031353373</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="4">
         <f>AVERAGEA(F2:F11)</f>
         <v>0.90820143014258181</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="4">
         <f>STDEV(F2:F11)</f>
         <v>7.0827513587667524E-3</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.908201430142582±0.00708275135876675</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="4">
         <f>AVERAGEA(N2:N11)</f>
         <v>0.72129238915688654</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="4">
         <f>STDEV(N2:N11)</f>
         <v>9.4957792854103266E-3</v>
       </c>
       <c r="L19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.721292389156887±0.00949577928541033</v>
+      </c>
+      <c r="R19" s="4">
+        <f>AVERAGEA(V2:V11)</f>
+        <v>0.9246400719555472</v>
+      </c>
+      <c r="S19" s="4">
+        <f>STDEV(V2:V11)</f>
+        <v>9.5631005523120465E-3</v>
+      </c>
+      <c r="T19" t="str">
+        <f t="shared" si="5"/>
+        <v>0.924640071955547±0.00956310055231205</v>
       </c>
     </row>
   </sheetData>
@@ -2762,10 +3281,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B01280E-4A82-453A-BE0E-B66BDEF08C4B}">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2775,7 +3294,7 @@
     <col min="7" max="7" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2812,568 +3331,626 @@
       <c r="N1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="Q1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1919</v>
+        <v>1976</v>
       </c>
       <c r="B2">
-        <v>1500</v>
+        <v>1851</v>
       </c>
       <c r="C2">
-        <v>2528486.9555358798</v>
+        <v>2915156.1804776099</v>
       </c>
       <c r="D2">
-        <v>1119369.2999112699</v>
+        <v>1603301.84266014</v>
       </c>
       <c r="E2">
-        <v>0.270195067273172</v>
+        <v>0.22029905677926301</v>
       </c>
       <c r="F2">
         <f>B2/A2</f>
-        <v>0.78165711307972907</v>
+        <v>0.93674089068825916</v>
       </c>
       <c r="I2">
-        <v>3900</v>
+        <v>4006</v>
       </c>
       <c r="J2">
-        <v>2421</v>
+        <v>2944</v>
       </c>
       <c r="K2">
-        <v>4642235.9914962603</v>
+        <v>4476441.7603266202</v>
       </c>
       <c r="L2">
-        <v>1591437.20218909</v>
+        <v>2405391.20685656</v>
       </c>
       <c r="M2">
-        <v>0.24067871242188499</v>
+        <v>0.20213145107894701</v>
       </c>
       <c r="N2">
         <f>J2/I2</f>
-        <v>0.62076923076923074</v>
+        <v>0.73489765351972047</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2">
-        <v>1032</v>
+        <v>1013</v>
       </c>
       <c r="R2">
-        <v>897</v>
+        <v>955</v>
       </c>
       <c r="S2">
-        <v>1439470.3240579299</v>
+        <v>1583144.70110797</v>
       </c>
       <c r="T2">
-        <v>691817.15730188601</v>
+        <v>869275.49049483205</v>
       </c>
       <c r="U2">
-        <v>0.23801808681915601</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+        <v>0.18803467093015699</v>
+      </c>
+      <c r="V2">
+        <f>R2/Q2</f>
+        <v>0.9427443237907206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1997</v>
+        <v>2014</v>
       </c>
       <c r="B3">
-        <v>1550</v>
+        <v>1876</v>
       </c>
       <c r="C3">
-        <v>2829717.6436582198</v>
+        <v>3069677.4207236101</v>
       </c>
       <c r="D3">
-        <v>1143390.6094819</v>
+        <v>1605538.8954826901</v>
       </c>
       <c r="E3">
-        <v>0.26848335122984501</v>
+        <v>0.20656190640154501</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F11" si="0">B3/A3</f>
-        <v>0.77616424636955428</v>
+        <v>0.93147964250248261</v>
       </c>
       <c r="I3">
-        <v>4002</v>
+        <v>4106</v>
       </c>
       <c r="J3">
-        <v>2513</v>
+        <v>3005</v>
       </c>
       <c r="K3">
-        <v>4813724.5762434499</v>
+        <v>4625726.65820836</v>
       </c>
       <c r="L3">
-        <v>1631177.9555464899</v>
+        <v>2366939.25818686</v>
       </c>
       <c r="M3">
-        <v>0.235714381559609</v>
+        <v>0.208219409545295</v>
       </c>
       <c r="N3">
         <f t="shared" ref="N3:N11" si="1">J3/I3</f>
-        <v>0.62793603198400805</v>
+        <v>0.73185582075012179</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3">
-        <v>981</v>
+        <v>957</v>
       </c>
       <c r="R3">
-        <v>841</v>
+        <v>907</v>
       </c>
       <c r="S3">
-        <v>1380949.24665707</v>
+        <v>1548087.2643452201</v>
       </c>
       <c r="T3">
-        <v>658181.87017437303</v>
+        <v>784925.54032745794</v>
       </c>
       <c r="U3">
-        <v>0.239940137258393</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+        <v>0.177528781768482</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V11" si="2">R3/Q3</f>
+        <v>0.94775339602925812</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>1969</v>
+        <v>2020</v>
       </c>
       <c r="B4">
-        <v>1532</v>
+        <v>1895</v>
       </c>
       <c r="C4">
-        <v>2812182.02186816</v>
+        <v>3113447.8922654302</v>
       </c>
       <c r="D4">
-        <v>1106506.8272408701</v>
+        <v>1612120.0801647</v>
       </c>
       <c r="E4">
-        <v>0.26892395743332398</v>
+        <v>0.22084319829134799</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>0.77805992889791775</v>
+        <v>0.93811881188118806</v>
       </c>
       <c r="I4">
-        <v>3923</v>
+        <v>4091</v>
       </c>
       <c r="J4">
-        <v>2510</v>
+        <v>3003</v>
       </c>
       <c r="K4">
-        <v>4964513.3908924405</v>
+        <v>4777082.7019759296</v>
       </c>
       <c r="L4">
-        <v>1694835.59956992</v>
+        <v>2329947.9647346898</v>
       </c>
       <c r="M4">
-        <v>0.236472859818666</v>
+        <v>0.19884977333388401</v>
       </c>
       <c r="N4">
         <f t="shared" si="1"/>
-        <v>0.63981646698954886</v>
+        <v>0.73405035443656808</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4">
-        <v>987</v>
+        <v>1013</v>
       </c>
       <c r="R4">
-        <v>858</v>
+        <v>938</v>
       </c>
       <c r="S4">
-        <v>1404586.4100506301</v>
+        <v>1572274.83847236</v>
       </c>
       <c r="T4">
-        <v>652913.29638775496</v>
+        <v>829977.143824197</v>
       </c>
       <c r="U4">
-        <v>0.24034136716055399</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+        <v>0.18284320563228701</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="2"/>
+        <v>0.92596248766041456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2055</v>
+        <v>2103</v>
       </c>
       <c r="B5">
-        <v>1587</v>
+        <v>1952</v>
       </c>
       <c r="C5">
-        <v>2930565.4836707101</v>
+        <v>3148961.2920267498</v>
       </c>
       <c r="D5">
-        <v>1146180.5402784201</v>
+        <v>1632751.8484235399</v>
       </c>
       <c r="E5">
-        <v>0.26835897847907098</v>
+        <v>0.219278626236378</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>0.77226277372262775</v>
+        <v>0.92819781264859724</v>
       </c>
       <c r="I5">
-        <v>4014</v>
+        <v>3967</v>
       </c>
       <c r="J5">
-        <v>2533</v>
+        <v>2875</v>
       </c>
       <c r="K5">
-        <v>4857893.6589313103</v>
+        <v>4524685.2915100399</v>
       </c>
       <c r="L5">
-        <v>1645122.1011069601</v>
+        <v>2262879.9177192301</v>
       </c>
       <c r="M5">
-        <v>0.22883208514163</v>
+        <v>0.212602408071555</v>
       </c>
       <c r="N5">
         <f t="shared" si="1"/>
-        <v>0.63104135525660188</v>
+        <v>0.72472901436854043</v>
       </c>
       <c r="P5" s="1"/>
       <c r="Q5">
-        <v>1046</v>
+        <v>1017</v>
       </c>
       <c r="R5">
-        <v>926</v>
+        <v>938</v>
       </c>
       <c r="S5">
-        <v>1614809.2406181099</v>
+        <v>1524207.3677531399</v>
       </c>
       <c r="T5">
-        <v>733600.86175208795</v>
+        <v>870519.28431084205</v>
       </c>
       <c r="U5">
-        <v>0.24447546631860601</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+        <v>0.18213854943050101</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="2"/>
+        <v>0.92232055063913476</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1921</v>
+        <v>2051</v>
       </c>
       <c r="B6">
-        <v>1538</v>
+        <v>1905</v>
       </c>
       <c r="C6">
-        <v>2648797.59578466</v>
+        <v>3000439.5151331299</v>
       </c>
       <c r="D6">
-        <v>1085971.24762413</v>
+        <v>1607532.03030256</v>
       </c>
       <c r="E6">
-        <v>0.26173616532819399</v>
+        <v>0.20581157805037301</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>0.80062467464862053</v>
+        <v>0.92881521209166262</v>
       </c>
       <c r="I6">
-        <v>3941</v>
+        <v>4057</v>
       </c>
       <c r="J6">
-        <v>2466</v>
+        <v>2919</v>
       </c>
       <c r="K6">
-        <v>4857649.06753485</v>
+        <v>4703283.6294500101</v>
       </c>
       <c r="L6">
-        <v>1638932.5948014499</v>
+        <v>2384059.3428972601</v>
       </c>
       <c r="M6">
-        <v>0.239687154203852</v>
+        <v>0.193319978423173</v>
       </c>
       <c r="N6">
         <f t="shared" si="1"/>
-        <v>0.62572951027657953</v>
+        <v>0.71949716539314768</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6">
-        <v>963</v>
+        <v>918</v>
       </c>
       <c r="R6">
-        <v>837</v>
+        <v>874</v>
       </c>
       <c r="S6">
-        <v>1424759.5286238701</v>
+        <v>1399620.5</v>
       </c>
       <c r="T6">
-        <v>693783.12383224</v>
+        <v>735040.40457227197</v>
       </c>
       <c r="U6">
-        <v>0.23003623706446</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+        <v>0.167200186847069</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="2"/>
+        <v>0.95206971677559915</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>1991</v>
+        <v>2056</v>
       </c>
       <c r="B7">
-        <v>1559</v>
+        <v>1901</v>
       </c>
       <c r="C7">
-        <v>3059085.5606007501</v>
+        <v>3149925.9886468002</v>
       </c>
       <c r="D7">
-        <v>1206641.07024212</v>
+        <v>1663190.80926992</v>
       </c>
       <c r="E7">
-        <v>0.27560396203292098</v>
+        <v>0.21746169764690901</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>0.78302360622802614</v>
+        <v>0.92461089494163429</v>
       </c>
       <c r="I7">
-        <v>4038</v>
+        <v>3964</v>
       </c>
       <c r="J7">
-        <v>2561</v>
+        <v>2978</v>
       </c>
       <c r="K7">
-        <v>5015355.4988432396</v>
+        <v>4673873.3532800004</v>
       </c>
       <c r="L7">
-        <v>1617725.71326449</v>
+        <v>2358926.9039191399</v>
       </c>
       <c r="M7">
-        <v>0.236171649931114</v>
+        <v>0.21251127436932499</v>
       </c>
       <c r="N7">
         <f t="shared" si="1"/>
-        <v>0.63422486379395737</v>
+        <v>0.75126135216952572</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7">
-        <v>1001</v>
+        <v>1008</v>
       </c>
       <c r="R7">
-        <v>876</v>
+        <v>927</v>
       </c>
       <c r="S7">
-        <v>1517453.91834706</v>
+        <v>1497914</v>
       </c>
       <c r="T7">
-        <v>672243.89858774596</v>
+        <v>806002.91994405002</v>
       </c>
       <c r="U7">
-        <v>0.23731842577251999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+        <v>0.183354062228653</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="2"/>
+        <v>0.9196428571428571</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2006</v>
+        <v>2053</v>
       </c>
       <c r="B8">
-        <v>1595</v>
+        <v>1918</v>
       </c>
       <c r="C8">
-        <v>2882334.1544772899</v>
+        <v>3162009.4090768602</v>
       </c>
       <c r="D8">
-        <v>1166255.34889995</v>
+        <v>1694415.59160464</v>
       </c>
       <c r="E8">
-        <v>0.26002034469247098</v>
+        <v>0.216833078106762</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>0.79511465603190423</v>
+        <v>0.93424257184607895</v>
       </c>
       <c r="I8">
-        <v>4040</v>
+        <v>4050</v>
       </c>
       <c r="J8">
-        <v>2572</v>
+        <v>2930</v>
       </c>
       <c r="K8">
-        <v>4938468.8657538798</v>
+        <v>4630155.6361101205</v>
       </c>
       <c r="L8">
-        <v>1642547.2489100201</v>
+        <v>2312170.3702435298</v>
       </c>
       <c r="M8">
-        <v>0.23752971358321201</v>
+        <v>0.20219704280286099</v>
       </c>
       <c r="N8">
         <f t="shared" si="1"/>
-        <v>0.63663366336633664</v>
+        <v>0.72345679012345676</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8">
-        <v>982</v>
+        <v>1019</v>
       </c>
       <c r="R8">
-        <v>854</v>
+        <v>956</v>
       </c>
       <c r="S8">
-        <v>1519421.21231526</v>
+        <v>1578769.7304219001</v>
       </c>
       <c r="T8">
-        <v>716381.070387732</v>
+        <v>873434.14867011702</v>
       </c>
       <c r="U8">
-        <v>0.25298317175149898</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+        <v>0.18811396485288101</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="2"/>
+        <v>0.93817468105986257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>1954</v>
+        <v>2007</v>
       </c>
       <c r="B9">
-        <v>1520</v>
+        <v>1854</v>
       </c>
       <c r="C9">
-        <v>2759398.9969905601</v>
+        <v>3071996.1977549698</v>
       </c>
       <c r="D9">
-        <v>1115652.2414756401</v>
+        <v>1598862.37094131</v>
       </c>
       <c r="E9">
-        <v>0.27130513602655398</v>
+        <v>0.215525931768005</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>0.77789150460593659</v>
+        <v>0.92376681614349776</v>
       </c>
       <c r="I9">
-        <v>3963</v>
+        <v>4092</v>
       </c>
       <c r="J9">
-        <v>2498</v>
+        <v>3006</v>
       </c>
       <c r="K9">
-        <v>4854489.1057365499</v>
+        <v>4693188.2966858698</v>
       </c>
       <c r="L9">
-        <v>1641116.8791634601</v>
+        <v>2356306.97939619</v>
       </c>
       <c r="M9">
-        <v>0.228146075640177</v>
+        <v>0.20015295007576001</v>
       </c>
       <c r="N9">
         <f t="shared" si="1"/>
-        <v>0.63033055765833967</v>
+        <v>0.73460410557184752</v>
       </c>
       <c r="P9" s="1"/>
       <c r="Q9">
-        <v>1067</v>
+        <v>1015</v>
       </c>
       <c r="R9">
-        <v>918</v>
+        <v>932</v>
       </c>
       <c r="S9">
-        <v>1672893.74405008</v>
+        <v>1460580.8180331001</v>
       </c>
       <c r="T9">
-        <v>766758.96038959105</v>
+        <v>761129.56399552699</v>
       </c>
       <c r="U9">
-        <v>0.25574322545914302</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+        <v>0.18625666380085101</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="2"/>
+        <v>0.91822660098522169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2006</v>
+        <v>2045</v>
       </c>
       <c r="B10">
-        <v>1532</v>
+        <v>1903</v>
       </c>
       <c r="C10">
-        <v>2889821.9653960401</v>
+        <v>3003729.3346260702</v>
       </c>
       <c r="D10">
-        <v>1191633.3966509299</v>
+        <v>1613980.9962994601</v>
       </c>
       <c r="E10">
-        <v>0.27740675527251402</v>
+        <v>0.20617672438548701</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>0.76370887337986038</v>
+        <v>0.93056234718826403</v>
       </c>
       <c r="I10">
-        <v>3995</v>
+        <v>3956</v>
       </c>
       <c r="J10">
-        <v>2577</v>
+        <v>2957</v>
       </c>
       <c r="K10">
-        <v>4811509.0961543797</v>
+        <v>4793885.0440102099</v>
       </c>
       <c r="L10">
-        <v>1629641.8871909501</v>
+        <v>2288675.4142384198</v>
       </c>
       <c r="M10">
-        <v>0.238212920657427</v>
+        <v>0.20669969366409</v>
       </c>
       <c r="N10">
         <f t="shared" si="1"/>
-        <v>0.64505632040050065</v>
+        <v>0.74747219413549038</v>
       </c>
       <c r="P10" s="1"/>
       <c r="Q10">
-        <v>975</v>
+        <v>984</v>
       </c>
       <c r="R10">
-        <v>832</v>
+        <v>919</v>
       </c>
       <c r="S10">
-        <v>1453942.7783506501</v>
+        <v>1432652.3798841201</v>
       </c>
       <c r="T10">
-        <v>689680.61972028203</v>
+        <v>777210.38590489305</v>
       </c>
       <c r="U10">
-        <v>0.24597337268443401</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+        <v>0.15602713954203501</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="2"/>
+        <v>0.93394308943089432</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2033</v>
+        <v>2026</v>
       </c>
       <c r="B11">
-        <v>1551</v>
+        <v>1834</v>
       </c>
       <c r="C11">
-        <v>2901361.9576620399</v>
+        <v>2983255.12584608</v>
       </c>
       <c r="D11">
-        <v>1151408.81268933</v>
+        <v>1568211.4946584301</v>
       </c>
       <c r="E11">
-        <v>0.26687573262631598</v>
+        <v>0.22054869709982</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>0.76291195277914414</v>
+        <v>0.90523198420533069</v>
       </c>
       <c r="I11">
-        <v>4015</v>
+        <v>4044</v>
       </c>
       <c r="J11">
-        <v>2571</v>
+        <v>2996</v>
       </c>
       <c r="K11">
-        <v>4902897.3146566702</v>
+        <v>4694396.6450161897</v>
       </c>
       <c r="L11">
-        <v>1635386.42877545</v>
+        <v>2350775.3033215702</v>
       </c>
       <c r="M11">
-        <v>0.23642449545713001</v>
+        <v>0.198010247555479</v>
       </c>
       <c r="N11">
         <f t="shared" si="1"/>
-        <v>0.64034869240348691</v>
+        <v>0.74085064292779423</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11">
-        <v>1024</v>
+        <v>1039</v>
       </c>
       <c r="R11">
-        <v>872</v>
+        <v>975</v>
       </c>
       <c r="S11">
-        <v>1523504.4772173699</v>
+        <v>1670037.64015007</v>
       </c>
       <c r="T11">
-        <v>724363.05735622195</v>
+        <v>939422.94959711202</v>
       </c>
       <c r="U11">
-        <v>0.24007147696206299</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+        <v>0.18668737145292799</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="2"/>
+        <v>0.93840230991337825</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -3381,120 +3958,168 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="4">
         <f>AVERAGEA(C2:C11)</f>
-        <v>2824175.2335644313</v>
-      </c>
-      <c r="C16">
+        <v>3061859.8356577316</v>
+      </c>
+      <c r="C16" s="4">
         <f>STDEV(A2:B2)</f>
-        <v>296.27774131716342</v>
-      </c>
-      <c r="D16" t="str">
+        <v>88.388347648318444</v>
+      </c>
+      <c r="D16" s="4" t="str">
         <f>B16&amp;"±"&amp;C16</f>
-        <v>2824175.23356443±296.277741317163</v>
-      </c>
-      <c r="J16">
+        <v>3061859.83565773±88.3883476483184</v>
+      </c>
+      <c r="J16" s="4">
         <f>AVERAGEA(K2:K11)</f>
-        <v>4865873.6566243032</v>
-      </c>
-      <c r="K16">
-        <f>STDEV(K2:K11)</f>
-        <v>102559.03637725826</v>
+        <v>4659271.9016573336</v>
+      </c>
+      <c r="K16" s="4">
+        <f>STDEV(I2:J2)</f>
+        <v>750.94740162011351</v>
       </c>
       <c r="L16" t="str">
         <f>J16&amp;"±"&amp;K16</f>
-        <v>4865873.6566243±102559.036377258</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+        <v>4659271.90165733±750.947401620114</v>
+      </c>
+      <c r="R16" s="4">
+        <f>AVERAGEA(S2:S11)</f>
+        <v>1526728.9240167879</v>
+      </c>
+      <c r="S16" s="4">
+        <f>STDEV(Q2:R2)</f>
+        <v>41.012193308819754</v>
+      </c>
+      <c r="T16" t="str">
+        <f>R16&amp;"±"&amp;S16</f>
+        <v>1526728.92401679±41.0121933088198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="4">
         <f>AVERAGEA(D2:D11)</f>
-        <v>1143300.9394494561</v>
-      </c>
-      <c r="C17">
+        <v>1619990.5959807388</v>
+      </c>
+      <c r="C17" s="4">
         <f>STDEV(D2:D11)</f>
-        <v>37898.424739977425</v>
-      </c>
-      <c r="D17" t="str">
-        <f t="shared" ref="D17:D19" si="2">B17&amp;"±"&amp;C17</f>
-        <v>1143300.93944946±37898.4247399774</v>
-      </c>
-      <c r="J17">
+        <v>35646.890925356471</v>
+      </c>
+      <c r="D17" s="4" t="str">
+        <f t="shared" ref="D17:D19" si="3">B17&amp;"±"&amp;C17</f>
+        <v>1619990.59598074±35646.8909253565</v>
+      </c>
+      <c r="J17" s="4">
         <f>AVERAGEA(L2:L11)</f>
-        <v>1636792.3610518281</v>
-      </c>
-      <c r="K17">
+        <v>2341607.2661513453</v>
+      </c>
+      <c r="K17" s="4">
         <f>STDEV(L2:L11)</f>
-        <v>25820.013476210544</v>
+        <v>43607.632548230213</v>
       </c>
       <c r="L17" t="str">
-        <f t="shared" ref="L17:L19" si="3">J17&amp;"±"&amp;K17</f>
-        <v>1636792.36105183±25820.0134762105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" ref="L17:L19" si="4">J17&amp;"±"&amp;K17</f>
+        <v>2341607.26615135±43607.6325482302</v>
+      </c>
+      <c r="R17" s="4">
+        <f>AVERAGEA(T2:T11)</f>
+        <v>824693.78316413006</v>
+      </c>
+      <c r="S17" s="4">
+        <f>STDEV(T2:T11)</f>
+        <v>63173.039886711274</v>
+      </c>
+      <c r="T17" t="str">
+        <f t="shared" ref="T17:T19" si="5">R17&amp;"±"&amp;S17</f>
+        <v>824693.78316413±63173.0398867113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="4">
         <f>AVERAGEA(E2:E11)</f>
-        <v>0.26889094503943817</v>
-      </c>
-      <c r="C18">
+        <v>0.21493404947658901</v>
+      </c>
+      <c r="C18" s="4">
         <f>STDEV(E2:E11)</f>
-        <v>5.3696926175061822E-3</v>
-      </c>
-      <c r="D18" t="str">
-        <f t="shared" si="2"/>
-        <v>0.268890945039438±0.00536969261750618</v>
-      </c>
-      <c r="J18">
+        <v>6.2756106850061907E-3</v>
+      </c>
+      <c r="D18" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>0.214934049476589±0.00627561068500619</v>
+      </c>
+      <c r="J18" s="4">
         <f>AVERAGEA(M2:M11)</f>
-        <v>0.23578700484147017</v>
-      </c>
-      <c r="K18">
+        <v>0.20346942289203684</v>
+      </c>
+      <c r="K18" s="4">
         <f>STDEV(M2:M11)</f>
-        <v>4.1612871114740674E-3</v>
+        <v>6.3833691114800533E-3</v>
       </c>
       <c r="L18" t="str">
-        <f t="shared" si="3"/>
-        <v>0.23578700484147±0.00416128711147407</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0.203469422892037±0.00638336911148005</v>
+      </c>
+      <c r="R18" s="4">
+        <f>AVERAGEA(U2:U11)</f>
+        <v>0.17981845964858437</v>
+      </c>
+      <c r="S18" s="4">
+        <f>STDEV(U2:U11)</f>
+        <v>1.0448161415434287E-2</v>
+      </c>
+      <c r="T18" t="str">
+        <f t="shared" si="5"/>
+        <v>0.179818459648584±0.0104481614154343</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="4">
         <f>AVERAGEA(F2:F11)</f>
-        <v>0.7791419329743321</v>
-      </c>
-      <c r="C19">
+        <v>0.92817669841369954</v>
+      </c>
+      <c r="C19" s="4">
         <f>STDEV(F2:F11)</f>
-        <v>1.2011776300153163E-2</v>
-      </c>
-      <c r="D19" t="str">
-        <f t="shared" si="2"/>
-        <v>0.779141932974332±0.0120117763001532</v>
-      </c>
-      <c r="J19">
+        <v>9.3370032154797659E-3</v>
+      </c>
+      <c r="D19" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>0.9281766984137±0.00933700321547977</v>
+      </c>
+      <c r="J19" s="4">
         <f>AVERAGEA(N2:N11)</f>
-        <v>0.63318866928985906</v>
-      </c>
-      <c r="K19">
+        <v>0.73426750933962137</v>
+      </c>
+      <c r="K19" s="4">
         <f>STDEV(N2:N11)</f>
-        <v>7.4478029879990141E-3</v>
+        <v>1.0213734848083507E-2</v>
       </c>
       <c r="L19" t="str">
-        <f t="shared" si="3"/>
-        <v>0.633188669289859±0.00744780298799901</v>
+        <f t="shared" si="4"/>
+        <v>0.734267509339621±0.0102137348480835</v>
+      </c>
+      <c r="R19" s="4">
+        <f>AVERAGEA(V2:V11)</f>
+        <v>0.93392400134273412</v>
+      </c>
+      <c r="S19" s="4">
+        <f>STDEV(V2:V11)</f>
+        <v>1.1948158157015875E-2</v>
+      </c>
+      <c r="T19" t="str">
+        <f t="shared" si="5"/>
+        <v>0.933924001342734±0.0119481581570159</v>
       </c>
     </row>
   </sheetData>
@@ -3506,10 +4131,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D87B97D5-C699-4D27-9F62-4625CCB6018E}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3529,10 +4154,10 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F1">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -3548,8 +4173,8 @@
       <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
-        <v>25</v>
+      <c r="E2" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -3565,8 +4190,8 @@
       <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
-        <v>26</v>
+      <c r="E3" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -3582,8 +4207,8 @@
       <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
-        <v>27</v>
+      <c r="E4" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -3599,73 +4224,1003 @@
       <c r="D5" t="s">
         <v>24</v>
       </c>
-      <c r="E5" t="s">
-        <v>28</v>
+      <c r="E5" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
       <c r="F6">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>38</v>
       </c>
       <c r="E7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
       <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>35</v>
       </c>
-      <c r="D8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
       <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
       <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>37</v>
       </c>
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="A1:E15">
+    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6729FCF2-885C-4371-BC79-30CEA04CB73B}">
+  <dimension ref="A1:P12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1375438.625</v>
+      </c>
+      <c r="B3">
+        <v>508313.53537580499</v>
+      </c>
+      <c r="C3">
+        <v>0.19440940678355501</v>
+      </c>
+      <c r="D3">
+        <v>0.76007677543186181</v>
+      </c>
+      <c r="E3">
+        <v>1527823.4749999901</v>
+      </c>
+      <c r="F3">
+        <v>698047.10983085597</v>
+      </c>
+      <c r="G3">
+        <v>0.189500472648126</v>
+      </c>
+      <c r="H3">
+        <v>0.89923224568138194</v>
+      </c>
+      <c r="I3">
+        <v>1412096.79514372</v>
+      </c>
+      <c r="J3">
+        <v>750253.49236876599</v>
+      </c>
+      <c r="K3">
+        <v>0.18791067091586899</v>
+      </c>
+      <c r="L3">
+        <v>0.93561786085150567</v>
+      </c>
+      <c r="M3">
+        <v>1583144.70110797</v>
+      </c>
+      <c r="N3">
+        <v>869275.49049483205</v>
+      </c>
+      <c r="O3">
+        <v>0.18803467093015699</v>
+      </c>
+      <c r="P3">
+        <f>L3/K3</f>
+        <v>4.9790565713556454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1439944.3249999899</v>
+      </c>
+      <c r="B4">
+        <v>492018.61660860502</v>
+      </c>
+      <c r="C4">
+        <v>0.18172517842192101</v>
+      </c>
+      <c r="D4">
+        <v>0.75815738963531665</v>
+      </c>
+      <c r="E4">
+        <v>1527823.4749999901</v>
+      </c>
+      <c r="F4">
+        <v>698047.10983085597</v>
+      </c>
+      <c r="G4">
+        <v>0.189500472648126</v>
+      </c>
+      <c r="H4">
+        <v>0.89923224568138194</v>
+      </c>
+      <c r="I4">
+        <v>1489496.0445817099</v>
+      </c>
+      <c r="J4">
+        <v>776786.83678934094</v>
+      </c>
+      <c r="K4">
+        <v>0.20416533663966499</v>
+      </c>
+      <c r="L4">
+        <v>0.9198355601233299</v>
+      </c>
+      <c r="M4">
+        <v>1548087.2643452201</v>
+      </c>
+      <c r="N4">
+        <v>784925.54032745794</v>
+      </c>
+      <c r="O4">
+        <v>0.177528781768482</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P12" si="0">L4/K4</f>
+        <v>4.5053463788848935</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1512929.8249999899</v>
+      </c>
+      <c r="B5">
+        <v>581303.68839501799</v>
+      </c>
+      <c r="C5">
+        <v>0.18260263406496399</v>
+      </c>
+      <c r="D5">
+        <v>0.76848249027237359</v>
+      </c>
+      <c r="E5">
+        <v>1634844.7250000001</v>
+      </c>
+      <c r="F5">
+        <v>802717.67269785295</v>
+      </c>
+      <c r="G5">
+        <v>0.20409025312008999</v>
+      </c>
+      <c r="H5">
+        <v>0.91828793774319062</v>
+      </c>
+      <c r="I5">
+        <v>1419744.24382972</v>
+      </c>
+      <c r="J5">
+        <v>758697.68235184206</v>
+      </c>
+      <c r="K5">
+        <v>0.188271171503227</v>
+      </c>
+      <c r="L5">
+        <v>0.92484342379958251</v>
+      </c>
+      <c r="M5">
+        <v>1572274.83847236</v>
+      </c>
+      <c r="N5">
+        <v>829977.143824197</v>
+      </c>
+      <c r="O5">
+        <v>0.18284320563228701</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>4.9122944124439707</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1524234.5</v>
+      </c>
+      <c r="B6">
+        <v>584156.74888740201</v>
+      </c>
+      <c r="C6">
+        <v>0.189200126990379</v>
+      </c>
+      <c r="D6">
+        <v>0.77626459143968873</v>
+      </c>
+      <c r="E6">
+        <v>1634844.7250000001</v>
+      </c>
+      <c r="F6">
+        <v>802717.67269785295</v>
+      </c>
+      <c r="G6">
+        <v>0.20409025312008999</v>
+      </c>
+      <c r="H6">
+        <v>0.91828793774319062</v>
+      </c>
+      <c r="I6">
+        <v>1456867.3336237599</v>
+      </c>
+      <c r="J6">
+        <v>742766.09569546301</v>
+      </c>
+      <c r="K6">
+        <v>0.20946071415717499</v>
+      </c>
+      <c r="L6">
+        <v>0.92315789473684207</v>
+      </c>
+      <c r="M6">
+        <v>1524207.3677531399</v>
+      </c>
+      <c r="N6">
+        <v>870519.28431084205</v>
+      </c>
+      <c r="O6">
+        <v>0.18213854943050101</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>4.4073080646718479</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1591181</v>
+      </c>
+      <c r="B7">
+        <v>592230.86057801102</v>
+      </c>
+      <c r="C7">
+        <v>0.211900232139585</v>
+      </c>
+      <c r="D7">
+        <v>0.75948196114708599</v>
+      </c>
+      <c r="E7">
+        <v>1732694.75</v>
+      </c>
+      <c r="F7">
+        <v>819445.85145720094</v>
+      </c>
+      <c r="G7">
+        <v>0.20102213679338099</v>
+      </c>
+      <c r="H7">
+        <v>0.92229417206290476</v>
+      </c>
+      <c r="I7">
+        <v>1525228.5626996099</v>
+      </c>
+      <c r="J7">
+        <v>809837.91777256306</v>
+      </c>
+      <c r="K7">
+        <v>0.19424720963258499</v>
+      </c>
+      <c r="L7">
+        <v>0.94094094094094094</v>
+      </c>
+      <c r="M7">
+        <v>1399620.5</v>
+      </c>
+      <c r="N7">
+        <v>735040.40457227197</v>
+      </c>
+      <c r="O7">
+        <v>0.167200186847069</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>4.8440383917005212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1505354.075</v>
+      </c>
+      <c r="B8">
+        <v>586052.43470445101</v>
+      </c>
+      <c r="C8">
+        <v>0.18973997598287101</v>
+      </c>
+      <c r="D8">
+        <v>0.72987974098057351</v>
+      </c>
+      <c r="E8">
+        <v>1732694.75</v>
+      </c>
+      <c r="F8">
+        <v>819445.85145720094</v>
+      </c>
+      <c r="G8">
+        <v>0.20102213679338099</v>
+      </c>
+      <c r="H8">
+        <v>0.92229417206290476</v>
+      </c>
+      <c r="I8">
+        <v>1472688.17189145</v>
+      </c>
+      <c r="J8">
+        <v>754291.10102044803</v>
+      </c>
+      <c r="K8">
+        <v>0.204147805857886</v>
+      </c>
+      <c r="L8">
+        <v>0.90861344537815125</v>
+      </c>
+      <c r="M8">
+        <v>1497914</v>
+      </c>
+      <c r="N8">
+        <v>806002.91994405002</v>
+      </c>
+      <c r="O8">
+        <v>0.183354062228653</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>4.4507627283080717</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1388277.3499999901</v>
+      </c>
+      <c r="B9">
+        <v>525776.65596643498</v>
+      </c>
+      <c r="C9">
+        <v>0.20433769927769299</v>
+      </c>
+      <c r="D9">
+        <v>0.73917421953675733</v>
+      </c>
+      <c r="E9">
+        <v>1529344.925</v>
+      </c>
+      <c r="F9">
+        <v>737490.01843370497</v>
+      </c>
+      <c r="G9">
+        <v>0.20199943397371101</v>
+      </c>
+      <c r="H9">
+        <v>0.90835850956696873</v>
+      </c>
+      <c r="I9">
+        <v>1540849.4251802501</v>
+      </c>
+      <c r="J9">
+        <v>769880.427347583</v>
+      </c>
+      <c r="K9">
+        <v>0.211465497033552</v>
+      </c>
+      <c r="L9">
+        <v>0.92162698412698407</v>
+      </c>
+      <c r="M9">
+        <v>1578769.7304219001</v>
+      </c>
+      <c r="N9">
+        <v>873434.14867011702</v>
+      </c>
+      <c r="O9">
+        <v>0.18811396485288101</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>4.3582853801476409</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1400052.95</v>
+      </c>
+      <c r="B10">
+        <v>523869.847428023</v>
+      </c>
+      <c r="C10">
+        <v>0.19867457442367001</v>
+      </c>
+      <c r="D10">
+        <v>0.75730110775427995</v>
+      </c>
+      <c r="E10">
+        <v>1529344.925</v>
+      </c>
+      <c r="F10">
+        <v>737490.01843370497</v>
+      </c>
+      <c r="G10">
+        <v>0.20199943397371101</v>
+      </c>
+      <c r="H10">
+        <v>0.90835850956696873</v>
+      </c>
+      <c r="I10">
+        <v>1492462.38796102</v>
+      </c>
+      <c r="J10">
+        <v>805823.69881653902</v>
+      </c>
+      <c r="K10">
+        <v>0.20595657710041301</v>
+      </c>
+      <c r="L10">
+        <v>0.91412213740458015</v>
+      </c>
+      <c r="M10">
+        <v>1460580.8180331001</v>
+      </c>
+      <c r="N10">
+        <v>761129.56399552699</v>
+      </c>
+      <c r="O10">
+        <v>0.18625666380085101</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>4.4384216822505493</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1441045.0249999999</v>
+      </c>
+      <c r="B11">
+        <v>531454.90064484498</v>
+      </c>
+      <c r="C11">
+        <v>0.178773811895486</v>
+      </c>
+      <c r="D11">
+        <v>0.75270935960591134</v>
+      </c>
+      <c r="E11">
+        <v>1565552.5999999901</v>
+      </c>
+      <c r="F11">
+        <v>741094.00191172597</v>
+      </c>
+      <c r="G11">
+        <v>0.20049069426036401</v>
+      </c>
+      <c r="H11">
+        <v>0.92413793103448272</v>
+      </c>
+      <c r="I11">
+        <v>1612738.73940765</v>
+      </c>
+      <c r="J11">
+        <v>860212.47909734095</v>
+      </c>
+      <c r="K11">
+        <v>0.20123133203839999</v>
+      </c>
+      <c r="L11">
+        <v>0.92884990253411304</v>
+      </c>
+      <c r="M11">
+        <v>1432652.3798841201</v>
+      </c>
+      <c r="N11">
+        <v>777210.38590489305</v>
+      </c>
+      <c r="O11">
+        <v>0.15602713954203501</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>4.6158314071929176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1448943.87499999</v>
+      </c>
+      <c r="B12">
+        <v>529757.85972009494</v>
+      </c>
+      <c r="C12">
+        <v>0.17646392516878101</v>
+      </c>
+      <c r="D12">
+        <v>0.76453201970443352</v>
+      </c>
+      <c r="E12">
+        <v>1565552.5999999901</v>
+      </c>
+      <c r="F12">
+        <v>741094.00191172597</v>
+      </c>
+      <c r="G12">
+        <v>0.20049069426036401</v>
+      </c>
+      <c r="H12">
+        <v>0.92413793103448272</v>
+      </c>
+      <c r="I12">
+        <v>1524664.9220285399</v>
+      </c>
+      <c r="J12">
+        <v>773561.49885178695</v>
+      </c>
+      <c r="K12">
+        <v>0.223996091016432</v>
+      </c>
+      <c r="L12">
+        <v>0.92879256965944268</v>
+      </c>
+      <c r="M12">
+        <v>1670037.64015007</v>
+      </c>
+      <c r="N12">
+        <v>939422.94959711202</v>
+      </c>
+      <c r="O12">
+        <v>0.18668737145292799</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>4.1464677595258035</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E7FEAB-E461-4CFC-87A9-E9E9C5D9B473}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0509344E-8C6D-4592-80E0-776EEF7BC7FC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7EC4068-7396-4F6F-B8B4-C4A75FE6989A}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2">
+        <v>1013</v>
+      </c>
+      <c r="C1">
+        <v>955</v>
+      </c>
+      <c r="D1">
+        <v>1583144.70110797</v>
+      </c>
+      <c r="E1">
+        <v>869275.49049483205</v>
+      </c>
+      <c r="F1">
+        <v>0.18803467093015699</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2">
+        <v>957</v>
+      </c>
+      <c r="C2">
+        <v>907</v>
+      </c>
+      <c r="D2">
+        <v>1548087.2643452201</v>
+      </c>
+      <c r="E2">
+        <v>784925.54032745794</v>
+      </c>
+      <c r="F2">
+        <v>0.177528781768482</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3">
+        <v>1013</v>
+      </c>
+      <c r="C3">
+        <v>938</v>
+      </c>
+      <c r="D3">
+        <v>1572274.83847236</v>
+      </c>
+      <c r="E3">
+        <v>829977.143824197</v>
+      </c>
+      <c r="F3">
+        <v>0.18284320563228701</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4">
+        <v>1017</v>
+      </c>
+      <c r="C4">
+        <v>938</v>
+      </c>
+      <c r="D4">
+        <v>1524207.3677531399</v>
+      </c>
+      <c r="E4">
+        <v>870519.28431084205</v>
+      </c>
+      <c r="F4">
+        <v>0.18213854943050101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5">
+        <v>918</v>
+      </c>
+      <c r="C5">
+        <v>874</v>
+      </c>
+      <c r="D5">
+        <v>1399620.5</v>
+      </c>
+      <c r="E5">
+        <v>735040.40457227197</v>
+      </c>
+      <c r="F5">
+        <v>0.167200186847069</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6">
+        <v>1008</v>
+      </c>
+      <c r="C6">
+        <v>927</v>
+      </c>
+      <c r="D6">
+        <v>1497914</v>
+      </c>
+      <c r="E6">
+        <v>806002.91994405002</v>
+      </c>
+      <c r="F6">
+        <v>0.183354062228653</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7">
+        <v>1019</v>
+      </c>
+      <c r="C7">
+        <v>956</v>
+      </c>
+      <c r="D7">
+        <v>1578769.7304219001</v>
+      </c>
+      <c r="E7">
+        <v>873434.14867011702</v>
+      </c>
+      <c r="F7">
+        <v>0.18811396485288101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8">
+        <v>1015</v>
+      </c>
+      <c r="C8">
+        <v>932</v>
+      </c>
+      <c r="D8">
+        <v>1460580.8180331001</v>
+      </c>
+      <c r="E8">
+        <v>761129.56399552699</v>
+      </c>
+      <c r="F8">
+        <v>0.18625666380085101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9">
+        <v>984</v>
+      </c>
+      <c r="C9">
+        <v>919</v>
+      </c>
+      <c r="D9">
+        <v>1432652.3798841201</v>
+      </c>
+      <c r="E9">
+        <v>777210.38590489305</v>
+      </c>
+      <c r="F9">
+        <v>0.15602713954203501</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10">
+        <v>1039</v>
+      </c>
+      <c r="C10">
+        <v>975</v>
+      </c>
+      <c r="D10">
+        <v>1670037.64015007</v>
+      </c>
+      <c r="E10">
+        <v>939422.94959711202</v>
+      </c>
+      <c r="F10">
+        <v>0.18668737145292799</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
vault backup: 2023-11-27 17:29:20
Affected files:
0. Attach/0.5 Archives/Evaluation Result.xlsx
1. Projects/2023-05-07 基于多智能体强化学习和反向拍卖机制的车联网任务调度/初稿-中文/5. 实验.md
</commit_message>
<xml_diff>
--- a/0. Attach/0.5 Archives/Evaluation Result.xlsx
+++ b/0. Attach/0.5 Archives/Evaluation Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuming\Documents\MateNote\0. Attach\0.5 Archives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51999DD-8987-4F04-AEFE-6C87EE3EF167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCC1E1E-207C-495C-BD2F-2758560181A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" activeTab="5" xr2:uid="{29E27A0B-FB5E-410D-B37C-BA3847E1800A}"/>
+    <workbookView xWindow="2057" yWindow="1423" windowWidth="24634" windowHeight="11023" activeTab="3" xr2:uid="{29E27A0B-FB5E-410D-B37C-BA3847E1800A}"/>
   </bookViews>
   <sheets>
     <sheet name="Random" sheetId="1" r:id="rId1"/>
@@ -23,72 +23,6 @@
     <sheet name="40" sheetId="9" r:id="rId8"/>
     <sheet name="Preparation" sheetId="6" r:id="rId9"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Random!$C$2:$C$11</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Random!$C$2:$C$30</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'10'!$A$10:$P$10</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'10'!$A$11:$P$11</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'10'!$A$12:$P$12</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'10'!$A$13:$P$13</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'10'!$A$14:$P$14</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'10'!$A$15:$P$15</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'10'!$A$16:$P$16</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'10'!$A$17:$P$17</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'10'!$A$18:$P$18</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'10'!$A$2:$P$2</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Random!$D$2:$D$11</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">'10'!$A$3:$P$3</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">'10'!$A$4:$P$4</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">'10'!$A$5:$P$5</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">'10'!$A$6:$P$6</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">'10'!$A$7:$P$7</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">'10'!$A$8:$P$8</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">'10'!$A$9:$P$9</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">'10'!$P$18</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">'10'!$A$10:$P$10</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">'10'!$A$11:$P$11</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Random!$D$2:$D$30</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">'10'!$A$12:$P$12</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">'10'!$A$13:$P$13</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">'10'!$A$14:$P$14</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">'10'!$A$15:$P$15</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">'10'!$A$16:$P$16</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">'10'!$A$17:$P$17</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">'10'!$A$18:$P$18</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">'10'!$A$2:$P$2</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">'10'!$A$3:$P$3</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">'10'!$A$4:$P$4</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Random!$E$2:$E$11</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">'10'!$A$5:$P$5</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">'10'!$A$6:$P$6</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">'10'!$A$7:$P$7</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">'10'!$A$8:$P$8</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">'10'!$A$9:$P$9</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">'10'!$P$18</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">'10'!$A$10:$P$10</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">'10'!$A$11:$P$11</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">'10'!$A$12:$P$12</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">'10'!$A$13:$P$13</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Random!$E$2:$E$30</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">'10'!$A$14:$P$14</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">'10'!$A$15:$P$15</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">'10'!$A$16:$P$16</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">'10'!$A$17:$P$17</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">'10'!$A$18:$P$18</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">'10'!$A$2:$P$2</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">'10'!$A$3:$P$3</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">'10'!$A$4:$P$4</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">'10'!$A$5:$P$5</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">'10'!$A$6:$P$6</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Random!$F$2:$F$11</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">'10'!$A$7:$P$7</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">'10'!$A$8:$P$8</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">'10'!$A$9:$P$9</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">'10'!$P$18</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Random!$F$2:$F$30</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Random!$F$30</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'10'!$P$18</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -110,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="64">
   <si>
     <t>Total Job</t>
   </si>
@@ -199,9 +133,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>4802908.625±99293.821642516</t>
-  </si>
-  <si>
     <t>1635198.84721598±34407.863752007</t>
   </si>
   <si>
@@ -211,9 +142,6 @@
     <t>0.629154787113477±0.00693142666753826</t>
   </si>
   <si>
-    <t>4732284.455±46297.6098102712</t>
-  </si>
-  <si>
     <t>2259543.11108798±33823.7058306808</t>
   </si>
   <si>
@@ -223,9 +151,6 @@
     <t>0.732066882151052±0.00938341815134694</t>
   </si>
   <si>
-    <t>4679116.6808595±95686.539654516</t>
-  </si>
-  <si>
     <t>2292832.59961928±53486.9772468569</t>
   </si>
   <si>
@@ -247,9 +172,6 @@
     <t>0.9281766984137±0.00933700321547977</t>
   </si>
   <si>
-    <t>4659271.90165733±100026.576065109</t>
-  </si>
-  <si>
     <t>2341607.26615135±43607.6325482302</t>
   </si>
   <si>
@@ -259,9 +181,6 @@
     <t>0.734267509339621±0.0102137348480835</t>
   </si>
   <si>
-    <t>1462740.155±69033.1420375868</t>
-  </si>
-  <si>
     <t>545493.514830869±36741.6904057123</t>
   </si>
   <si>
@@ -271,9 +190,6 @@
     <t>0.756605965550828±0.0135272734535628</t>
   </si>
   <si>
-    <t>1598052.095±81909.5620785324</t>
-  </si>
-  <si>
     <t>759758.930866268±47283.1068698491</t>
   </si>
   <si>
@@ -283,9 +199,6 @@
     <t>0.914462159217786±0.00987479813764537</t>
   </si>
   <si>
-    <t>1494683.66263474±59890.9885505285</t>
-  </si>
-  <si>
     <t>780211.123011167±35794.0092236306</t>
   </si>
   <si>
@@ -293,9 +206,6 @@
   </si>
   <si>
     <t>0.924640071955547±0.00956310055231205</t>
-  </si>
-  <si>
-    <t>1526728.92401679±81088.5388601975</t>
   </si>
   <si>
     <t>824693.78316413±63173.0398867113</t>
@@ -312,6 +222,30 @@
   <si>
     <t>PPO_LTSM</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4802908.625±1003.38452250371</t>
+  </si>
+  <si>
+    <t>1462740.155±176.776695296637</t>
+  </si>
+  <si>
+    <t>4732284.455±707.106781186548</t>
+  </si>
+  <si>
+    <t>1598052.095±74.2462120245875</t>
+  </si>
+  <si>
+    <t>4679116.6808595±773.574818618083</t>
+  </si>
+  <si>
+    <t>1494683.66263474±43.8406204335659</t>
+  </si>
+  <si>
+    <t>4659271.90165733±750.947401620114</t>
+  </si>
+  <si>
+    <t>1526728.92401679±41.0121933088198</t>
   </si>
 </sst>
 </file>
@@ -398,7 +332,97 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -737,16 +761,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEB75B47-34C0-4D1B-A289-611307C156F5}">
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:V11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.35546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -802,7 +826,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1951</v>
       </c>
@@ -862,7 +886,7 @@
         <v>0.76007677543186181</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1951</v>
       </c>
@@ -922,7 +946,7 @@
         <v>0.75815738963531665</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2040</v>
       </c>
@@ -982,7 +1006,7 @@
         <v>0.76848249027237359</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2040</v>
       </c>
@@ -1042,7 +1066,7 @@
         <v>0.77626459143968873</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2064</v>
       </c>
@@ -1102,7 +1126,7 @@
         <v>0.75948196114708599</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2064</v>
       </c>
@@ -1162,7 +1186,7 @@
         <v>0.72987974098057351</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1976</v>
       </c>
@@ -1222,7 +1246,7 @@
         <v>0.73917421953675733</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1976</v>
       </c>
@@ -1282,7 +1306,7 @@
         <v>0.75730110775427995</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1952</v>
       </c>
@@ -1342,7 +1366,7 @@
         <v>0.75270935960591134</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1952</v>
       </c>
@@ -1402,7 +1426,7 @@
         <v>0.76453201970443352</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -1410,7 +1434,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1451,7 +1475,7 @@
         <v>1462740.155±176.776695296637</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1492,7 +1516,7 @@
         <v>545493.514830869±36741.6904057123</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1533,7 +1557,7 @@
         <v>0.190782756514891±0.011580191640062</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1586,12 +1610,12 @@
   <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:V11"/>
+      <selection activeCell="T16" sqref="T16:T19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1647,7 +1671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1951</v>
       </c>
@@ -1707,7 +1731,7 @@
         <v>0.89923224568138194</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1951</v>
       </c>
@@ -1767,7 +1791,7 @@
         <v>0.89923224568138194</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2040</v>
       </c>
@@ -1827,7 +1851,7 @@
         <v>0.91828793774319062</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2040</v>
       </c>
@@ -1887,7 +1911,7 @@
         <v>0.91828793774319062</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2064</v>
       </c>
@@ -1947,7 +1971,7 @@
         <v>0.92229417206290476</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2064</v>
       </c>
@@ -2007,7 +2031,7 @@
         <v>0.92229417206290476</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1976</v>
       </c>
@@ -2067,7 +2091,7 @@
         <v>0.90835850956696873</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1976</v>
       </c>
@@ -2127,7 +2151,7 @@
         <v>0.90835850956696873</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1952</v>
       </c>
@@ -2187,7 +2211,7 @@
         <v>0.92413793103448272</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1952</v>
       </c>
@@ -2247,7 +2271,7 @@
         <v>0.92413793103448272</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -2255,7 +2279,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -2296,7 +2320,7 @@
         <v>1598052.095±74.2462120245875</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -2337,7 +2361,7 @@
         <v>759758.930866268±47283.1068698491</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -2378,7 +2402,7 @@
         <v>0.199420598159134±0.00538671191049339</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -2431,20 +2455,20 @@
   <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:V11"/>
+      <selection activeCell="T16" sqref="T16:T19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.35546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.35546875" customWidth="1"/>
+    <col min="5" max="5" width="12.35546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2500,7 +2524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1937</v>
       </c>
@@ -2560,7 +2584,7 @@
         <v>0.93561786085150567</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1982</v>
       </c>
@@ -2620,7 +2644,7 @@
         <v>0.9198355601233299</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2031</v>
       </c>
@@ -2680,7 +2704,7 @@
         <v>0.92484342379958251</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2026</v>
       </c>
@@ -2740,7 +2764,7 @@
         <v>0.92315789473684207</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1989</v>
       </c>
@@ -2800,7 +2824,7 @@
         <v>0.94094094094094094</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1995</v>
       </c>
@@ -2860,7 +2884,7 @@
         <v>0.90861344537815125</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2079</v>
       </c>
@@ -2920,7 +2944,7 @@
         <v>0.92162698412698407</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1951</v>
       </c>
@@ -2980,7 +3004,7 @@
         <v>0.91412213740458015</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2024</v>
       </c>
@@ -3040,7 +3064,7 @@
         <v>0.92884990253411304</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1960</v>
       </c>
@@ -3100,7 +3124,7 @@
         <v>0.92879256965944268</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -3108,7 +3132,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -3149,7 +3173,7 @@
         <v>1494683.66263474±43.8406204335659</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -3190,7 +3214,7 @@
         <v>780211.123011167±35794.0092236306</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -3231,7 +3255,7 @@
         <v>0.20308524058952±0.0110048031353373</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -3283,18 +3307,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B01280E-4A82-453A-BE0E-B66BDEF08C4B}">
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:V11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16:T19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3350,7 +3374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1976</v>
       </c>
@@ -3410,7 +3434,7 @@
         <v>0.9427443237907206</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2014</v>
       </c>
@@ -3470,7 +3494,7 @@
         <v>0.94775339602925812</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -3530,7 +3554,7 @@
         <v>0.92596248766041456</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2103</v>
       </c>
@@ -3590,7 +3614,7 @@
         <v>0.92232055063913476</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2051</v>
       </c>
@@ -3650,7 +3674,7 @@
         <v>0.95206971677559915</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2056</v>
       </c>
@@ -3710,7 +3734,7 @@
         <v>0.9196428571428571</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2053</v>
       </c>
@@ -3770,7 +3794,7 @@
         <v>0.93817468105986257</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2007</v>
       </c>
@@ -3830,7 +3854,7 @@
         <v>0.91822660098522169</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2045</v>
       </c>
@@ -3890,7 +3914,7 @@
         <v>0.93394308943089432</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2026</v>
       </c>
@@ -3950,7 +3974,7 @@
         <v>0.93840230991337825</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -3958,7 +3982,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -3999,7 +4023,7 @@
         <v>1526728.92401679±41.0121933088198</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -4040,7 +4064,7 @@
         <v>824693.78316413±63173.0398867113</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -4081,7 +4105,7 @@
         <v>0.179818459648584±0.0104481614154343</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -4134,16 +4158,16 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="39.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="39.2109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>10</v>
       </c>
@@ -4160,7 +4184,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -4174,10 +4198,10 @@
         <v>21</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -4191,10 +4215,10 @@
         <v>22</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -4208,10 +4232,10 @@
         <v>23</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -4225,10 +4249,10 @@
         <v>24</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -4245,75 +4269,75 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -4330,78 +4354,78 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D13" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="D15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A1:E15">
-    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="15" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4412,16 +4436,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6729FCF2-885C-4371-BC79-30CEA04CB73B}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4432,10 +4456,10 @@
         <v>12</v>
       </c>
       <c r="M1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4446,7 +4470,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -4458,7 +4482,7 @@
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="I2" t="s">
         <v>2</v>
@@ -4470,7 +4494,7 @@
         <v>4</v>
       </c>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="M2" t="s">
         <v>2</v>
@@ -4485,7 +4509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1375438.625</v>
       </c>
@@ -4536,7 +4560,7 @@
         <v>4.9790565713556454</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1439944.3249999899</v>
       </c>
@@ -4587,7 +4611,7 @@
         <v>4.5053463788848935</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1512929.8249999899</v>
       </c>
@@ -4638,7 +4662,7 @@
         <v>4.9122944124439707</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1524234.5</v>
       </c>
@@ -4689,7 +4713,7 @@
         <v>4.4073080646718479</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1591181</v>
       </c>
@@ -4740,7 +4764,7 @@
         <v>4.8440383917005212</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1505354.075</v>
       </c>
@@ -4791,7 +4815,7 @@
         <v>4.4507627283080717</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1388277.3499999901</v>
       </c>
@@ -4842,7 +4866,7 @@
         <v>4.3582853801476409</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1400052.95</v>
       </c>
@@ -4893,7 +4917,7 @@
         <v>4.4384216822505493</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1441045.0249999999</v>
       </c>
@@ -4944,7 +4968,7 @@
         <v>4.6158314071929176</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1448943.87499999</v>
       </c>
@@ -5007,7 +5031,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5020,7 +5044,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5029,197 +5053,274 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7EC4068-7396-4F6F-B8B4-C4A75FE6989A}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F10"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="3" width="34.78515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.92578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2">
-        <v>1013</v>
-      </c>
-      <c r="C1">
-        <v>955</v>
-      </c>
-      <c r="D1">
-        <v>1583144.70110797</v>
-      </c>
-      <c r="E1">
-        <v>869275.49049483205</v>
-      </c>
-      <c r="F1">
-        <v>0.18803467093015699</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2">
-        <v>957</v>
-      </c>
-      <c r="C2">
-        <v>907</v>
-      </c>
-      <c r="D2">
-        <v>1548087.2643452201</v>
-      </c>
-      <c r="E2">
-        <v>784925.54032745794</v>
-      </c>
-      <c r="F2">
-        <v>0.177528781768482</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3">
-        <v>1013</v>
-      </c>
-      <c r="C3">
-        <v>938</v>
-      </c>
-      <c r="D3">
-        <v>1572274.83847236</v>
-      </c>
-      <c r="E3">
-        <v>829977.143824197</v>
-      </c>
-      <c r="F3">
-        <v>0.18284320563228701</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4">
-        <v>1017</v>
-      </c>
-      <c r="C4">
-        <v>938</v>
-      </c>
-      <c r="D4">
-        <v>1524207.3677531399</v>
-      </c>
-      <c r="E4">
-        <v>870519.28431084205</v>
-      </c>
-      <c r="F4">
-        <v>0.18213854943050101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5">
-        <v>918</v>
-      </c>
-      <c r="C5">
-        <v>874</v>
-      </c>
-      <c r="D5">
-        <v>1399620.5</v>
-      </c>
-      <c r="E5">
-        <v>735040.40457227197</v>
-      </c>
-      <c r="F5">
-        <v>0.167200186847069</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
-      <c r="B6">
-        <v>1008</v>
-      </c>
-      <c r="C6">
-        <v>927</v>
-      </c>
-      <c r="D6">
-        <v>1497914</v>
-      </c>
-      <c r="E6">
-        <v>806002.91994405002</v>
-      </c>
-      <c r="F6">
-        <v>0.183354062228653</v>
-      </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
-      <c r="B7">
-        <v>1019</v>
-      </c>
-      <c r="C7">
-        <v>956</v>
-      </c>
-      <c r="D7">
-        <v>1578769.7304219001</v>
-      </c>
-      <c r="E7">
-        <v>873434.14867011702</v>
-      </c>
-      <c r="F7">
-        <v>0.18811396485288101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
-      <c r="B8">
-        <v>1015</v>
-      </c>
-      <c r="C8">
-        <v>932</v>
-      </c>
-      <c r="D8">
-        <v>1460580.8180331001</v>
-      </c>
-      <c r="E8">
-        <v>761129.56399552699</v>
-      </c>
-      <c r="F8">
-        <v>0.18625666380085101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
-      <c r="B9">
-        <v>984</v>
-      </c>
-      <c r="C9">
-        <v>919</v>
-      </c>
-      <c r="D9">
-        <v>1432652.3798841201</v>
-      </c>
-      <c r="E9">
-        <v>777210.38590489305</v>
-      </c>
-      <c r="F9">
-        <v>0.15602713954203501</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
-      <c r="B10">
-        <v>1039</v>
-      </c>
-      <c r="C10">
-        <v>975</v>
-      </c>
-      <c r="D10">
-        <v>1670037.64015007</v>
-      </c>
-      <c r="E10">
-        <v>939422.94959711202</v>
-      </c>
-      <c r="F10">
-        <v>0.18668737145292799</v>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="A1:J5">
+    <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:G12">
+    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>